<commit_message>
Error en mostrar lista de cargos a trabajadores
</commit_message>
<xml_diff>
--- a/Documentacion y Planeacion de Trabajo/Sprint Backlog _Pila del Sprint.xlsx
+++ b/Documentacion y Planeacion de Trabajo/Sprint Backlog _Pila del Sprint.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="9240"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de Usuario" sheetId="1" r:id="rId1"/>
@@ -1049,11 +1049,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BQ143"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G13" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="77" zoomScaleNormal="100" zoomScaleSheetLayoutView="77" workbookViewId="0">
+      <pane xSplit="6" ySplit="5" topLeftCell="G22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2763,7 +2763,7 @@
         <v>62</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G15" s="5">
         <v>4</v>
@@ -2911,7 +2911,7 @@
         <v>65</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G16" s="5">
         <v>2</v>
@@ -3057,7 +3057,7 @@
         <v>52</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G17" s="5">
         <v>3</v>
@@ -3205,7 +3205,7 @@
         <v>52</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G18" s="5">
         <v>3</v>
@@ -3343,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:69" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
       <c r="D19" s="5" t="s">
@@ -3353,7 +3353,7 @@
         <v>65</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G19" s="5">
         <v>2</v>
@@ -3505,7 +3505,7 @@
         <v>62</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G20" s="5">
         <v>3</v>
@@ -3653,7 +3653,7 @@
         <v>55</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G21" s="5">
         <v>2</v>
@@ -3801,7 +3801,7 @@
         <v>55</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G22" s="5">
         <v>2</v>
@@ -4091,7 +4091,7 @@
         <v>52</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="G24" s="5">
         <v>1</v>
@@ -4677,7 +4677,7 @@
         <v>62</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G28" s="5">
         <v>3</v>
@@ -5263,7 +5263,7 @@
         <v>62</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G32" s="5">
         <v>4</v>
@@ -5851,7 +5851,7 @@
         <v>62</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G36" s="5">
         <v>3</v>
@@ -7625,7 +7625,7 @@
         <v>65</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G48" s="5">
         <v>1</v>
@@ -7765,7 +7765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:69" ht="30" x14ac:dyDescent="0.25">
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
       <c r="D49" s="5" t="s">
@@ -7775,7 +7775,7 @@
         <v>55</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G49" s="5">
         <v>2</v>
@@ -7915,7 +7915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:69" ht="30" x14ac:dyDescent="0.25">
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
       <c r="D50" s="5" t="s">
@@ -7925,7 +7925,7 @@
         <v>55</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="G50" s="5">
         <v>1</v>
@@ -22079,6 +22079,72 @@
     </row>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="AL4:AM4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AF4:AG4"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="BG4:BH4"/>
+    <mergeCell ref="BJ4:BK4"/>
+    <mergeCell ref="BM4:BN4"/>
+    <mergeCell ref="BP4:BQ4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
+    <mergeCell ref="BA4:BB4"/>
+    <mergeCell ref="BD4:BE4"/>
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="C76:C79"/>
+    <mergeCell ref="C80:C83"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="C88:C91"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="C92:C95"/>
+    <mergeCell ref="B92:B95"/>
+    <mergeCell ref="C97:C99"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="B112:B115"/>
+    <mergeCell ref="C116:C119"/>
+    <mergeCell ref="B116:B119"/>
+    <mergeCell ref="C100:C103"/>
+    <mergeCell ref="B100:B103"/>
+    <mergeCell ref="B104:B107"/>
+    <mergeCell ref="C104:C107"/>
+    <mergeCell ref="C108:C111"/>
+    <mergeCell ref="B108:B111"/>
     <mergeCell ref="C132:C135"/>
     <mergeCell ref="B132:B135"/>
     <mergeCell ref="C136:C139"/>
@@ -22095,72 +22161,6 @@
     <mergeCell ref="B128:B131"/>
     <mergeCell ref="C128:C131"/>
     <mergeCell ref="C112:C115"/>
-    <mergeCell ref="B112:B115"/>
-    <mergeCell ref="C116:C119"/>
-    <mergeCell ref="B116:B119"/>
-    <mergeCell ref="C100:C103"/>
-    <mergeCell ref="B100:B103"/>
-    <mergeCell ref="B104:B107"/>
-    <mergeCell ref="C104:C107"/>
-    <mergeCell ref="C108:C111"/>
-    <mergeCell ref="B108:B111"/>
-    <mergeCell ref="C88:C91"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="C92:C95"/>
-    <mergeCell ref="B92:B95"/>
-    <mergeCell ref="C97:C99"/>
-    <mergeCell ref="B96:B99"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="C76:C79"/>
-    <mergeCell ref="C80:C83"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="C14:C19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="BG4:BH4"/>
-    <mergeCell ref="BJ4:BK4"/>
-    <mergeCell ref="BM4:BN4"/>
-    <mergeCell ref="BP4:BQ4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
-    <mergeCell ref="BA4:BB4"/>
-    <mergeCell ref="BD4:BE4"/>
-    <mergeCell ref="AL4:AM4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AF4:AG4"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="B64:B67"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="53" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Arreglando bugs trabajadores,terrenos crud completo; falta organizar empezar dia
</commit_message>
<xml_diff>
--- a/Documentacion y Planeacion de Trabajo/Sprint Backlog _Pila del Sprint.xlsx
+++ b/Documentacion y Planeacion de Trabajo/Sprint Backlog _Pila del Sprint.xlsx
@@ -1050,10 +1050,10 @@
   <dimension ref="B1:BQ143"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="77" zoomScaleNormal="100" zoomScaleSheetLayoutView="77" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C32" sqref="C32:C35"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,7 +1431,7 @@
         <v>52</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>53</v>
+        <v>151</v>
       </c>
       <c r="G6" s="5">
         <v>3</v>
@@ -2911,7 +2911,7 @@
         <v>65</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>53</v>
+        <v>151</v>
       </c>
       <c r="G16" s="5">
         <v>2</v>
@@ -3057,7 +3057,7 @@
         <v>52</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>53</v>
+        <v>151</v>
       </c>
       <c r="G17" s="5">
         <v>3</v>
@@ -3205,7 +3205,7 @@
         <v>52</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>53</v>
+        <v>151</v>
       </c>
       <c r="G18" s="5">
         <v>3</v>
@@ -3343,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:69" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
       <c r="D19" s="5" t="s">
@@ -3353,7 +3353,7 @@
         <v>65</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>53</v>
+        <v>151</v>
       </c>
       <c r="G19" s="5">
         <v>2</v>
@@ -4239,7 +4239,7 @@
         <v>65</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G25" s="5">
         <v>1</v>
@@ -4387,7 +4387,7 @@
         <v>65</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G26" s="5">
         <v>1</v>
@@ -4825,7 +4825,7 @@
         <v>65</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G29" s="5">
         <v>1</v>
@@ -4973,7 +4973,7 @@
         <v>65</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G30" s="5">
         <v>1</v>
@@ -5413,7 +5413,7 @@
         <v>55</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G33" s="5">
         <v>2</v>
@@ -5561,7 +5561,7 @@
         <v>55</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="G34" s="5">
         <v>2</v>
@@ -5851,7 +5851,7 @@
         <v>62</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>53</v>
+        <v>151</v>
       </c>
       <c r="G36" s="5">
         <v>3</v>
@@ -5991,7 +5991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:69" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
       <c r="D37" s="5" t="s">
@@ -6001,7 +6001,7 @@
         <v>65</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G37" s="5">
         <v>2</v>
@@ -6141,7 +6141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:69" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:69" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
       <c r="D38" s="5" t="s">
@@ -6151,7 +6151,7 @@
         <v>65</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G38" s="5">
         <v>2</v>
@@ -6443,7 +6443,7 @@
         <v>52</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G40" s="5">
         <v>2</v>
@@ -6593,7 +6593,7 @@
         <v>55</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G41" s="5">
         <v>1</v>
@@ -6741,7 +6741,7 @@
         <v>52</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G42" s="5">
         <v>2</v>
@@ -7033,7 +7033,7 @@
         <v>52</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G44" s="5">
         <v>1</v>
@@ -7183,7 +7183,7 @@
         <v>65</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G45" s="5">
         <v>1</v>
@@ -7333,7 +7333,7 @@
         <v>65</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="G46" s="5">
         <v>1</v>
@@ -7625,7 +7625,7 @@
         <v>65</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>151</v>
+        <v>53</v>
       </c>
       <c r="G48" s="5">
         <v>1</v>
@@ -22079,6 +22079,72 @@
     </row>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="AL4:AM4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AF4:AG4"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="BG4:BH4"/>
+    <mergeCell ref="BJ4:BK4"/>
+    <mergeCell ref="BM4:BN4"/>
+    <mergeCell ref="BP4:BQ4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
+    <mergeCell ref="BA4:BB4"/>
+    <mergeCell ref="BD4:BE4"/>
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="C76:C79"/>
+    <mergeCell ref="C80:C83"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="C88:C91"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="C92:C95"/>
+    <mergeCell ref="B92:B95"/>
+    <mergeCell ref="C97:C99"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="B112:B115"/>
+    <mergeCell ref="C116:C119"/>
+    <mergeCell ref="B116:B119"/>
+    <mergeCell ref="C100:C103"/>
+    <mergeCell ref="B100:B103"/>
+    <mergeCell ref="B104:B107"/>
+    <mergeCell ref="C104:C107"/>
+    <mergeCell ref="C108:C111"/>
+    <mergeCell ref="B108:B111"/>
     <mergeCell ref="C132:C135"/>
     <mergeCell ref="B132:B135"/>
     <mergeCell ref="C136:C139"/>
@@ -22095,72 +22161,6 @@
     <mergeCell ref="B128:B131"/>
     <mergeCell ref="C128:C131"/>
     <mergeCell ref="C112:C115"/>
-    <mergeCell ref="B112:B115"/>
-    <mergeCell ref="C116:C119"/>
-    <mergeCell ref="B116:B119"/>
-    <mergeCell ref="C100:C103"/>
-    <mergeCell ref="B100:B103"/>
-    <mergeCell ref="B104:B107"/>
-    <mergeCell ref="C104:C107"/>
-    <mergeCell ref="C108:C111"/>
-    <mergeCell ref="B108:B111"/>
-    <mergeCell ref="C88:C91"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="C92:C95"/>
-    <mergeCell ref="B92:B95"/>
-    <mergeCell ref="C97:C99"/>
-    <mergeCell ref="B96:B99"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="C76:C79"/>
-    <mergeCell ref="C80:C83"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="C14:C19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="BG4:BH4"/>
-    <mergeCell ref="BJ4:BK4"/>
-    <mergeCell ref="BM4:BN4"/>
-    <mergeCell ref="BP4:BQ4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
-    <mergeCell ref="BA4:BB4"/>
-    <mergeCell ref="BD4:BE4"/>
-    <mergeCell ref="AL4:AM4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AF4:AG4"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="B64:B67"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="53" orientation="landscape" r:id="rId1"/>

</xml_diff>